<commit_message>
Essential splice variants demoted from score=4 to score=3 (now same as missense)
</commit_message>
<xml_diff>
--- a/data/variant_significance/sig_scoring.xlsx
+++ b/data/variant_significance/sig_scoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lnguyen/hpc/cog_bioinf/cuppen/project_data/Luan_projects/CHORD/scripts_main/hmfGeneAnnotation/data/variant_significance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B2109C-1730-6844-8065-39C54BE1DD18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D259F62-24F2-A947-93C3-6BC53B6F630B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="32900" windowHeight="20560" activeTab="1" xr2:uid="{A59E393C-A626-AF48-9EE9-279A0D857A2F}"/>
+    <workbookView xWindow="39420" yWindow="-3140" windowWidth="32900" windowHeight="20540" activeTab="1" xr2:uid="{A59E393C-A626-AF48-9EE9-279A0D857A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="snpeff" sheetId="3" r:id="rId1"/>
@@ -27,6 +27,12 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1630,7 +1636,7 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G57"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1865,8 +1871,7 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <f>IF(ISNUMBER(C10),C10,"")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>110</v>
@@ -1887,8 +1892,7 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <f>IF(ISNUMBER(C11),C11,"")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>110</v>

</xml_diff>